<commit_message>
Incorporación de Footy Stats DB
</commit_message>
<xml_diff>
--- a/Twitter/03_18_05_2022_Liguilla_MX_Semis_1/Soporte_03_18_05_2022.xlsx
+++ b/Twitter/03_18_05_2022_Liguilla_MX_Semis_1/Soporte_03_18_05_2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\La Cima del Éxito\Futbol\Twitter\03_18_05_2022_Liguilla_MX_Semis_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB7F1D69-D66E-4FF2-9315-D7982F66243A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE2793D-1391-48A1-8F6F-5AEA22C6FFB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{F233A4A7-37D6-4F23-935B-2462791656C2}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" activeTab="1" xr2:uid="{F233A4A7-37D6-4F23-935B-2462791656C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Atlas_Tigres_ida" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <definedName name="Margin">Atlas_Tigres_ida!$G$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="64">
   <si>
     <t>Atlas</t>
   </si>
@@ -224,13 +225,23 @@
   <si>
     <t>Sevilla</t>
   </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -275,13 +286,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -847,7 +859,17 @@
           </a:p>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
@@ -2625,7 +2647,14 @@
           </a:p>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
             </a:pPr>
             <a:r>
               <a:rPr lang="es-MX"/>
@@ -6262,8 +6291,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A2:H82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6553,7 +6582,7 @@
         <v>6</v>
       </c>
       <c r="D30" s="2">
-        <f>1/C30</f>
+        <f t="shared" ref="D30:D58" si="1">1/C30</f>
         <v>0.16666666666666666</v>
       </c>
       <c r="E30">
@@ -6571,7 +6600,7 @@
         <v>6.5</v>
       </c>
       <c r="D31" s="4">
-        <f>1/C31</f>
+        <f t="shared" si="1"/>
         <v>0.15384615384615385</v>
       </c>
       <c r="E31">
@@ -6589,7 +6618,7 @@
         <v>6.5</v>
       </c>
       <c r="D32" s="2">
-        <f>1/C32</f>
+        <f t="shared" si="1"/>
         <v>0.15384615384615385</v>
       </c>
       <c r="E32">
@@ -6607,7 +6636,7 @@
         <v>6</v>
       </c>
       <c r="D33" s="2">
-        <f>1/C33</f>
+        <f t="shared" si="1"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="E33">
@@ -6625,7 +6654,7 @@
         <v>12</v>
       </c>
       <c r="D34" s="4">
-        <f>1/C34</f>
+        <f t="shared" si="1"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="E34">
@@ -6643,7 +6672,7 @@
         <v>12</v>
       </c>
       <c r="D35" s="2">
-        <f>1/C35</f>
+        <f t="shared" si="1"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="E35">
@@ -6661,7 +6690,7 @@
         <v>29</v>
       </c>
       <c r="D36" s="4">
-        <f>1/C36</f>
+        <f t="shared" si="1"/>
         <v>3.4482758620689655E-2</v>
       </c>
       <c r="E36">
@@ -6679,7 +6708,7 @@
         <v>29</v>
       </c>
       <c r="D37" s="2">
-        <f>1/C37</f>
+        <f t="shared" si="1"/>
         <v>3.4482758620689655E-2</v>
       </c>
       <c r="E37">
@@ -6697,7 +6726,7 @@
         <v>11</v>
       </c>
       <c r="D38" s="4">
-        <f>1/C38</f>
+        <f t="shared" si="1"/>
         <v>9.0909090909090912E-2</v>
       </c>
       <c r="E38">
@@ -6715,7 +6744,7 @@
         <v>11</v>
       </c>
       <c r="D39" s="2">
-        <f>1/C39</f>
+        <f t="shared" si="1"/>
         <v>9.0909090909090912E-2</v>
       </c>
       <c r="E39">
@@ -6733,7 +6762,7 @@
         <v>67</v>
       </c>
       <c r="D40" s="2">
-        <f>1/C40</f>
+        <f t="shared" si="1"/>
         <v>1.4925373134328358E-2</v>
       </c>
       <c r="E40">
@@ -6751,7 +6780,7 @@
         <v>67</v>
       </c>
       <c r="D41" s="2">
-        <f>1/C41</f>
+        <f t="shared" si="1"/>
         <v>1.4925373134328358E-2</v>
       </c>
       <c r="E41">
@@ -6769,7 +6798,7 @@
         <v>29</v>
       </c>
       <c r="D42" s="2">
-        <f>1/C42</f>
+        <f t="shared" si="1"/>
         <v>3.4482758620689655E-2</v>
       </c>
       <c r="E42">
@@ -6787,7 +6816,7 @@
         <v>29</v>
       </c>
       <c r="D43" s="2">
-        <f>1/C43</f>
+        <f t="shared" si="1"/>
         <v>3.4482758620689655E-2</v>
       </c>
       <c r="E43">
@@ -6805,7 +6834,7 @@
         <v>19</v>
       </c>
       <c r="D44" s="2">
-        <f>1/C44</f>
+        <f t="shared" si="1"/>
         <v>5.2631578947368418E-2</v>
       </c>
       <c r="E44">
@@ -6823,7 +6852,7 @@
         <v>201</v>
       </c>
       <c r="D45" s="2">
-        <f>1/C45</f>
+        <f t="shared" si="1"/>
         <v>4.9751243781094526E-3</v>
       </c>
       <c r="E45">
@@ -6841,7 +6870,7 @@
         <v>67</v>
       </c>
       <c r="D46" s="2">
-        <f>1/C46</f>
+        <f t="shared" si="1"/>
         <v>1.4925373134328358E-2</v>
       </c>
       <c r="E46">
@@ -6859,7 +6888,7 @@
         <v>67</v>
       </c>
       <c r="D47" s="2">
-        <f>1/C47</f>
+        <f t="shared" si="1"/>
         <v>1.4925373134328358E-2</v>
       </c>
       <c r="E47">
@@ -6877,7 +6906,7 @@
         <v>41</v>
       </c>
       <c r="D48" s="2">
-        <f>1/C48</f>
+        <f t="shared" si="1"/>
         <v>2.4390243902439025E-2</v>
       </c>
       <c r="E48">
@@ -6895,7 +6924,7 @@
         <v>41</v>
       </c>
       <c r="D49" s="2">
-        <f>1/C49</f>
+        <f t="shared" si="1"/>
         <v>2.4390243902439025E-2</v>
       </c>
       <c r="E49">
@@ -6913,7 +6942,7 @@
         <v>201</v>
       </c>
       <c r="D50" s="2">
-        <f>1/C50</f>
+        <f t="shared" si="1"/>
         <v>4.9751243781094526E-3</v>
       </c>
       <c r="E50">
@@ -6931,7 +6960,7 @@
         <v>201</v>
       </c>
       <c r="D51" s="2">
-        <f>1/C51</f>
+        <f t="shared" si="1"/>
         <v>4.9751243781094526E-3</v>
       </c>
       <c r="E51">
@@ -6949,7 +6978,7 @@
         <v>101</v>
       </c>
       <c r="D52" s="2">
-        <f>1/C52</f>
+        <f t="shared" si="1"/>
         <v>9.9009900990099011E-3</v>
       </c>
       <c r="E52">
@@ -6967,7 +6996,7 @@
         <v>101</v>
       </c>
       <c r="D53" s="2">
-        <f>1/C53</f>
+        <f t="shared" si="1"/>
         <v>9.9009900990099011E-3</v>
       </c>
       <c r="E53">
@@ -6985,7 +7014,7 @@
         <v>81</v>
       </c>
       <c r="D54" s="2">
-        <f>1/C54</f>
+        <f t="shared" si="1"/>
         <v>1.2345679012345678E-2</v>
       </c>
       <c r="E54">
@@ -7003,7 +7032,7 @@
         <v>351</v>
       </c>
       <c r="D55" s="2">
-        <f>1/C55</f>
+        <f t="shared" si="1"/>
         <v>2.8490028490028491E-3</v>
       </c>
       <c r="E55">
@@ -7021,7 +7050,7 @@
         <v>351</v>
       </c>
       <c r="D56" s="2">
-        <f>1/C56</f>
+        <f t="shared" si="1"/>
         <v>2.8490028490028491E-3</v>
       </c>
       <c r="E56">
@@ -7039,7 +7068,7 @@
         <v>201</v>
       </c>
       <c r="D57" s="2">
-        <f>1/C57</f>
+        <f t="shared" si="1"/>
         <v>4.9751243781094526E-3</v>
       </c>
       <c r="E57">
@@ -7057,7 +7086,7 @@
         <v>201</v>
       </c>
       <c r="D58" s="2">
-        <f>1/C58</f>
+        <f t="shared" si="1"/>
         <v>4.9751243781094526E-3</v>
       </c>
       <c r="E58">
@@ -7205,15 +7234,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27566A6C-97A0-4F90-AFF0-A29F7A2C853C}">
-  <dimension ref="B2:F23"/>
+  <dimension ref="B2:N23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>54</v>
       </c>
@@ -7223,8 +7252,17 @@
       <c r="D2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="J2" t="s">
+        <v>61</v>
+      </c>
+      <c r="K2" t="s">
+        <v>62</v>
+      </c>
+      <c r="L2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B3">
         <v>2.4</v>
       </c>
@@ -7234,8 +7272,20 @@
       <c r="D3">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="J3">
+        <v>1.5</v>
+      </c>
+      <c r="K3">
+        <v>5</v>
+      </c>
+      <c r="L3">
+        <v>7.5</v>
+      </c>
+      <c r="N3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B4">
         <f>1/B3</f>
         <v>0.41666666666666669</v>
@@ -7252,8 +7302,51 @@
         <f>(SUM(B4:D4)-1)/3</f>
         <v>1.7676767676767662E-2</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="J4">
+        <f>1/J3</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="K4">
+        <f t="shared" ref="K4:L4" si="1">1/K3</f>
+        <v>0.2</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="1"/>
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="N4" s="6">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="J5">
+        <f>J4+$N$4/3</f>
+        <v>0.69333333333333325</v>
+      </c>
+      <c r="K5">
+        <f t="shared" ref="K5:L5" si="2">K4+$N$4/3</f>
+        <v>0.22666666666666668</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="2"/>
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="J6">
+        <f>1/J5</f>
+        <v>1.4423076923076925</v>
+      </c>
+      <c r="K6">
+        <f t="shared" ref="K6:L6" si="3">1/K5</f>
+        <v>4.4117647058823524</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="3"/>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
         <v>54</v>
       </c>
@@ -7264,21 +7357,21 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B8" s="1">
         <f>B4-$F$4</f>
         <v>0.39898989898989901</v>
       </c>
       <c r="C8" s="1">
-        <f t="shared" ref="C8:D8" si="1">C4-$F$4</f>
+        <f t="shared" ref="C8:D8" si="4">C4-$F$4</f>
         <v>0.28535353535353536</v>
       </c>
       <c r="D8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.31565656565656564</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
         <v>57</v>
       </c>
@@ -7289,7 +7382,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B12">
         <v>2.1</v>
       </c>
@@ -7300,17 +7393,17 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B13">
         <f>1/B12</f>
         <v>0.47619047619047616</v>
       </c>
       <c r="C13">
-        <f t="shared" ref="C13:D13" si="2">1/C12</f>
+        <f t="shared" ref="C13:D13" si="5">1/C12</f>
         <v>0.30769230769230771</v>
       </c>
       <c r="D13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.27777777777777779</v>
       </c>
       <c r="F13">
@@ -7318,7 +7411,7 @@
         <v>2.0553520553520555E-2</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B16" t="s">
         <v>57</v>
       </c>
@@ -7335,11 +7428,11 @@
         <v>0.45563695563695561</v>
       </c>
       <c r="C17" s="1">
-        <f t="shared" ref="C17:D17" si="3">C13-$F$13</f>
+        <f t="shared" ref="C17:D17" si="6">C13-$F$13</f>
         <v>0.28713878713878715</v>
       </c>
       <c r="D17" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.25722425722425724</v>
       </c>
       <c r="F17">
@@ -7375,11 +7468,11 @@
         <v>0.36363636363636365</v>
       </c>
       <c r="C22">
-        <f t="shared" ref="C22:D22" si="4">1/C21</f>
+        <f t="shared" ref="C22:D22" si="7">1/C21</f>
         <v>0.30303030303030304</v>
       </c>
       <c r="D22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.38461538461538458</v>
       </c>
       <c r="F22">
@@ -7393,11 +7486,11 @@
         <v>0.34654234654234656</v>
       </c>
       <c r="C23" s="1">
-        <f t="shared" ref="C23:D23" si="5">C22-$F$22</f>
+        <f t="shared" ref="C23:D23" si="8">C22-$F$22</f>
         <v>0.28593628593628595</v>
       </c>
       <c r="D23" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.36752136752136749</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Añadido el Tweet con reporte de Partido de ida final Clausura2020
</commit_message>
<xml_diff>
--- a/Twitter/03_18_05_2022_Liguilla_MX_Semis_1/Soporte_03_18_05_2022.xlsx
+++ b/Twitter/03_18_05_2022_Liguilla_MX_Semis_1/Soporte_03_18_05_2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\La Cima del Éxito\Futbol\Twitter\03_18_05_2022_Liguilla_MX_Semis_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE2793D-1391-48A1-8F6F-5AEA22C6FFB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48430442-FF0C-445A-AAA1-607F190DB35D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" activeTab="1" xr2:uid="{F233A4A7-37D6-4F23-935B-2462791656C2}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{F233A4A7-37D6-4F23-935B-2462791656C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Atlas_Tigres_ida" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,6 @@
     <definedName name="Margin">Atlas_Tigres_ida!$G$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -6291,8 +6290,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A2:H82"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7236,7 +7235,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27566A6C-97A0-4F90-AFF0-A29F7A2C853C}">
   <dimension ref="B2:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>

</xml_diff>